<commit_message>
Feat: incluir arquivo de autenticação
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henrique.ls\Desktop\RPAs\Templates_CoE\Suzano_ReFramework_Queue_v23.4\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41790A1C-7FEF-4B31-96AB-288F7FC09CBF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -30,189 +46,204 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Asset</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>System exception.</t>
-  </si>
-  <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>RPA0180</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Gerencia de Energia/Matriz Energetica/ProcessamentoDeFaturas</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>RPA ID</t>
+  </si>
+  <si>
+    <t>AzureApp_Secret_Credential</t>
+  </si>
+  <si>
+    <t>StorageBucket</t>
+  </si>
+  <si>
+    <t>RPA0180-Files</t>
+  </si>
+  <si>
+    <t>StorageBucketDirectoryPath</t>
+  </si>
+  <si>
+    <t>MaxRetryNumber</t>
+  </si>
+  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>ExScreenshotsFolderPath</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_Success</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
     <t>Static part of logging message. Processed Transaction succesful.</t>
   </si>
   <si>
+    <t>LogMessage_Success_CoE</t>
+  </si>
+  <si>
+    <t>[COECSS-SUCESSO]</t>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException</t>
+  </si>
+  <si>
+    <t>Business rule exception.</t>
+  </si>
+  <si>
     <t>Static part of logging message. Processed Transaction failed with business exception.</t>
   </si>
   <si>
+    <t>LogMessage_ApplicationException</t>
+  </si>
+  <si>
+    <t>System exception.</t>
+  </si>
+  <si>
     <t>Static part of logging message. Processed Transaction failed with application exception.</t>
   </si>
   <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t>Asset</t>
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
-    <t>LogMessage_Success_CoE</t>
-  </si>
-  <si>
-    <t>[COECSS-SUCESSO]</t>
-  </si>
-  <si>
-    <t>TRUE</t>
+    <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>PathVideoRecorder</t>
+  </si>
+  <si>
+    <t>R_QA_VIDEOS</t>
+  </si>
+  <si>
+    <t>Shared Asset - Folder Path where recordered video will salved</t>
+  </si>
+  <si>
+    <t>FFmpegFilePath</t>
+  </si>
+  <si>
+    <t>R_QA_FFMPEG</t>
+  </si>
+  <si>
+    <t>Shared Asset - FFMPEG.exe file path</t>
+  </si>
+  <si>
+    <t>DesktopVideoRecorder</t>
+  </si>
+  <si>
+    <t>Used to determine if robots will recorder the execution or not</t>
+  </si>
+  <si>
+    <t>AzureApp_ApplicationID</t>
+  </si>
+  <si>
+    <t>AzureApp_Tenant</t>
+  </si>
+  <si>
+    <t>TeamID</t>
+  </si>
+  <si>
+    <t>RPA0157_TeamsID_Channel</t>
   </si>
   <si>
     <t>ApplicationsProcessesNames</t>
-  </si>
-  <si>
-    <t>List of applications processes names separate by common used in this automation. This information is used in Kill All Applications Workflow as Arrays Of String</t>
-  </si>
-  <si>
-    <t>RPA000x</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>RPA ID</t>
-  </si>
-  <si>
-    <t>DesktopVideoRecorder</t>
-  </si>
-  <si>
-    <t>PathVideoRecorder</t>
-  </si>
-  <si>
-    <t>FFmpegFilePath</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>Used to determine if robots will recorder the execution or not</t>
-  </si>
-  <si>
-    <t>Recorder_PATH_VIDEOS</t>
-  </si>
-  <si>
-    <t>Shared Asset - Folder Path where recordered video will salved</t>
-  </si>
-  <si>
-    <t>Recorder_PATH_FFMPEG_EXE</t>
-  </si>
-  <si>
-    <t>Shared Asset - FFMPEG.exe file path</t>
-  </si>
-  <si>
-    <t>Shared</t>
-  </si>
-  <si>
-    <t>saplogon</t>
   </si>
 </sst>
 </file>
@@ -289,9 +320,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -329,7 +360,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -435,7 +466,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -577,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -586,18 +617,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="141" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -608,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -636,57 +667,77 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.8">
+    <row r="3" spans="1:26" ht="30">
       <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.4">
+    <row r="4" spans="1:26">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.4">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1674,9 +1725,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1690,15 +1738,15 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="59.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="139.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="139.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1709,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1735,151 +1783,151 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.4">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:3" ht="14.4">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2865,15 +2913,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2881,13 +2929,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2914,27 +2962,27 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
-        <v>61</v>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
@@ -2942,18 +2990,51 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
+        <v>61</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Feat: Obtem as crecenciais para MS e Google
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41790A1C-7FEF-4B31-96AB-288F7FC09CBF}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FA2F045-E168-489F-B400-4DF4E6D7B41E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,15 @@
     <t>StorageBucketDirectoryPath</t>
   </si>
   <si>
+    <t>ApplicationsProcessesNames</t>
+  </si>
+  <si>
+    <t>GCPDataSet</t>
+  </si>
+  <si>
+    <t>RPA0180_ODBC</t>
+  </si>
+  <si>
     <t>MaxRetryNumber</t>
   </si>
   <si>
@@ -241,9 +250,6 @@
   </si>
   <si>
     <t>RPA0157_TeamsID_Channel</t>
-  </si>
-  <si>
-    <t>ApplicationsProcessesNames</t>
   </si>
 </sst>
 </file>
@@ -320,9 +326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -360,7 +366,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -466,7 +472,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -608,7 +614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,7 +626,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -735,11 +741,18 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1785,149 +1798,149 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2929,13 +2942,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2962,52 +2975,52 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -3015,10 +3028,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -3026,10 +3039,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
fix: configurando download do json
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FA2F045-E168-489F-B400-4DF4E6D7B41E}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B875445-6955-4859-9665-77B64DC86714}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>RPA0180_ODBC</t>
+  </si>
+  <si>
+    <t>Local_PDF</t>
+  </si>
+  <si>
+    <t>C:\COE_Files\RPA0180\PDF_files</t>
+  </si>
+  <si>
+    <t>Local_JSON</t>
+  </si>
+  <si>
+    <t>C:\COE_Files\RPA0180\Json_files</t>
   </si>
   <si>
     <t>MaxRetryNumber</t>
@@ -626,7 +638,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -753,8 +765,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1798,149 +1824,149 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2942,13 +2968,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2975,52 +3001,52 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -3028,10 +3054,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -3039,10 +3065,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Fix: Incluindo notificação via teams caso seja substituta
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B875445-6955-4859-9665-77B64DC86714}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BA2213E-0A98-4B5D-AC5E-AF2F87DA6B0E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>RPA0157_TeamsID_Channel</t>
+  </si>
+  <si>
+    <t>WordsKeys</t>
+  </si>
+  <si>
+    <t>RPA0180_Word_Keys</t>
+  </si>
+  <si>
+    <t>Palavras chave para verificar se a fatura é substituta</t>
   </si>
 </sst>
 </file>
@@ -2952,7 +2961,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3074,7 +3083,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix:  incluindo salvamento de dados no GCP fields principais
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BA2213E-0A98-4B5D-AC5E-AF2F87DA6B0E}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E84D86E9-6E2A-46BD-9E4E-6F8AE8525938}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -264,13 +264,22 @@
     <t>RPA0157_TeamsID_Channel</t>
   </si>
   <si>
-    <t>WordsKeys</t>
-  </si>
-  <si>
-    <t>RPA0180_Word_Keys</t>
+    <t>WordsKeys_Subs</t>
+  </si>
+  <si>
+    <t>RPA0180_Word_Keys_Subs</t>
   </si>
   <si>
     <t>Palavras chave para verificar se a fatura é substituta</t>
+  </si>
+  <si>
+    <t>WordsKeys_Titular</t>
+  </si>
+  <si>
+    <t>RPA0180_Word_Keys_Titular</t>
+  </si>
+  <si>
+    <t>Palavras chave para verificar se fatura pertence ao grupo suzano ou terceiro</t>
   </si>
 </sst>
 </file>
@@ -322,11 +331,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -646,7 +658,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2960,8 +2972,8 @@
   <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3097,7 +3109,20 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: download master data e consulta instalação - v 1.0.1
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E84D86E9-6E2A-46BD-9E4E-6F8AE8525938}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BBC5AD4-4A8C-41CC-BB1A-571CB4511F5E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>C:\COE_Files\RPA0180\Json_files</t>
+  </si>
+  <si>
+    <t>StorageBucketName</t>
+  </si>
+  <si>
+    <t>RPA0174-Files</t>
   </si>
   <si>
     <t>MaxRetryNumber</t>
@@ -658,8 +664,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -802,7 +808,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1845,149 +1858,149 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2972,7 +2985,7 @@
   <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2989,13 +3002,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3022,52 +3035,52 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -3075,10 +3088,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -3086,10 +3099,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -3097,30 +3110,30 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Enviando dados de fatura e masterdata para fila do RPA0174 v: 1.0.2
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BBC5AD4-4A8C-41CC-BB1A-571CB4511F5E}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00636CA5-B185-47BD-A327-C5006A120B5D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>RPA0174-Files</t>
+  </si>
+  <si>
+    <t>QueueName</t>
+  </si>
+  <si>
+    <t>RPA0174</t>
+  </si>
+  <si>
+    <t>Local_JSON_Export</t>
+  </si>
+  <si>
+    <t>C:\COE_Files\RPA0180\Json_files_exp</t>
   </si>
   <si>
     <t>MaxRetryNumber</t>
@@ -665,7 +677,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -816,8 +828,22 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1858,149 +1884,149 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3002,13 +3028,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3035,52 +3061,52 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -3088,10 +3114,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -3099,10 +3125,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -3110,30 +3136,30 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Atualização de notificação via teams v: 1.0.6
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00636CA5-B185-47BD-A327-C5006A120B5D}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D41C6485-691D-48F0-A788-574E14765248}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -228,6 +228,12 @@
     <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
   </si>
   <si>
+    <t>MaxMailsToBeRetrivied</t>
+  </si>
+  <si>
+    <t>RPA0180_MaxMailsToBeRetrivied</t>
+  </si>
+  <si>
     <t>ShouldMarkJobAsFaulted</t>
   </si>
   <si>
@@ -298,6 +304,18 @@
   </si>
   <si>
     <t>Palavras chave para verificar se fatura pertence ao grupo suzano ou terceiro</t>
+  </si>
+  <si>
+    <t>TableGCP</t>
+  </si>
+  <si>
+    <t>RPA0180_TableGCP</t>
+  </si>
+  <si>
+    <t>Substitui datasetGCP na query SQL para o nome do dataset correto</t>
+  </si>
+  <si>
+    <t>Define a quantidade de tentativas em caso de falha</t>
   </si>
 </sst>
 </file>
@@ -377,9 +395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -417,7 +435,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -523,7 +541,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -665,7 +683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -676,7 +694,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1834,10 +1852,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2017,18 +2035,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>64</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
     </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2999,7 +3017,6 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3012,7 +3029,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3028,13 +3045,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3061,52 +3078,52 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -3114,10 +3131,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -3125,10 +3142,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -3136,34 +3153,60 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix? Correção URL fatura sharepoint v:1.0.7
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D41C6485-691D-48F0-A788-574E14765248}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CABA95EF-371A-4D5C-A8EC-5636D538FDC4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -228,94 +228,100 @@
     <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
   </si>
   <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>PathVideoRecorder</t>
+  </si>
+  <si>
+    <t>R_QA_VIDEOS</t>
+  </si>
+  <si>
+    <t>Shared Asset - Folder Path where recordered video will salved</t>
+  </si>
+  <si>
+    <t>FFmpegFilePath</t>
+  </si>
+  <si>
+    <t>R_QA_FFMPEG</t>
+  </si>
+  <si>
+    <t>Shared Asset - FFMPEG.exe file path</t>
+  </si>
+  <si>
+    <t>DesktopVideoRecorder</t>
+  </si>
+  <si>
+    <t>Used to determine if robots will recorder the execution or not</t>
+  </si>
+  <si>
+    <t>AzureApp_ApplicationID</t>
+  </si>
+  <si>
+    <t>AzureApp_Tenant</t>
+  </si>
+  <si>
+    <t>TeamID</t>
+  </si>
+  <si>
+    <t>RPA0157_TeamsID_Channel</t>
+  </si>
+  <si>
+    <t>WordsKeys_Subs</t>
+  </si>
+  <si>
+    <t>RPA0180_Word_Keys_Subs</t>
+  </si>
+  <si>
+    <t>Palavras chave para verificar se a fatura é substituta</t>
+  </si>
+  <si>
+    <t>WordsKeys_Titular</t>
+  </si>
+  <si>
+    <t>RPA0180_Word_Keys_Titular</t>
+  </si>
+  <si>
+    <t>Palavras chave para verificar se fatura pertence ao grupo suzano ou terceiro</t>
+  </si>
+  <si>
+    <t>TableGCP</t>
+  </si>
+  <si>
+    <t>RPA0180_TableGCP</t>
+  </si>
+  <si>
+    <t>Substitui datasetGCP na query SQL para o nome do dataset correto</t>
+  </si>
+  <si>
     <t>MaxMailsToBeRetrivied</t>
   </si>
   <si>
     <t>RPA0180_MaxMailsToBeRetrivied</t>
   </si>
   <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>PathVideoRecorder</t>
-  </si>
-  <si>
-    <t>R_QA_VIDEOS</t>
-  </si>
-  <si>
-    <t>Shared Asset - Folder Path where recordered video will salved</t>
-  </si>
-  <si>
-    <t>FFmpegFilePath</t>
-  </si>
-  <si>
-    <t>R_QA_FFMPEG</t>
-  </si>
-  <si>
-    <t>Shared Asset - FFMPEG.exe file path</t>
-  </si>
-  <si>
-    <t>DesktopVideoRecorder</t>
-  </si>
-  <si>
-    <t>Used to determine if robots will recorder the execution or not</t>
-  </si>
-  <si>
-    <t>AzureApp_ApplicationID</t>
-  </si>
-  <si>
-    <t>AzureApp_Tenant</t>
-  </si>
-  <si>
-    <t>TeamID</t>
-  </si>
-  <si>
-    <t>RPA0157_TeamsID_Channel</t>
-  </si>
-  <si>
-    <t>WordsKeys_Subs</t>
-  </si>
-  <si>
-    <t>RPA0180_Word_Keys_Subs</t>
-  </si>
-  <si>
-    <t>Palavras chave para verificar se a fatura é substituta</t>
-  </si>
-  <si>
-    <t>WordsKeys_Titular</t>
-  </si>
-  <si>
-    <t>RPA0180_Word_Keys_Titular</t>
-  </si>
-  <si>
-    <t>Palavras chave para verificar se fatura pertence ao grupo suzano ou terceiro</t>
-  </si>
-  <si>
-    <t>TableGCP</t>
-  </si>
-  <si>
-    <t>RPA0180_TableGCP</t>
-  </si>
-  <si>
-    <t>Substitui datasetGCP na query SQL para o nome do dataset correto</t>
-  </si>
-  <si>
     <t>Define a quantidade de tentativas em caso de falha</t>
+  </si>
+  <si>
+    <t>URL_Sharepoint</t>
+  </si>
+  <si>
+    <t>SharepoiintEnergia</t>
   </si>
 </sst>
 </file>
@@ -395,9 +401,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -435,7 +441,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -541,7 +547,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -683,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1854,7 +1860,7 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2037,13 +2043,13 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
         <v>64</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3028,8 +3034,8 @@
   <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3045,13 +3051,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3078,52 +3084,52 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -3131,10 +3137,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -3142,10 +3148,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -3153,52 +3159,52 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
@@ -3207,7 +3213,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Comentando atividade do teams para teste em QA v: 1.1.3
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CABA95EF-371A-4D5C-A8EC-5636D538FDC4}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE364330-152F-43B1-8F28-D0F571B0FA6E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -3035,7 +3035,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3115,7 +3115,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Feat: Ajuste nos assets do arquivo config e nome arquivos de fila v: 1.1.8
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE364330-152F-43B1-8F28-D0F571B0FA6E}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B902189F-16F9-4FB0-9D39-E1273D35D33D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3035,7 +3035,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3115,7 +3115,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Feat: Ajuste nas credenciais do google v: 1.1.9
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B902189F-16F9-4FB0-9D39-E1273D35D33D}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6121314C-5B50-45C0-83B3-FC6F88534735}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -97,12 +97,6 @@
   </si>
   <si>
     <t>ApplicationsProcessesNames</t>
-  </si>
-  <si>
-    <t>GCPDataSet</t>
-  </si>
-  <si>
-    <t>RPA0180_ODBC</t>
   </si>
   <si>
     <t>Local_PDF</t>
@@ -698,10 +692,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -837,18 +831,18 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
     </row>
@@ -860,14 +854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1847,7 +1834,6 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1908,148 +1894,148 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
         <v>49</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
         <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3051,13 +3037,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3084,52 +3070,52 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -3137,10 +3123,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -3148,10 +3134,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -3159,66 +3145,66 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Fix: validando quando é e-mail de retorno da area para faturas substitutas v1.3.3
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/Suzano/AUTOMACOES/RPA0180/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6121314C-5B50-45C0-83B3-FC6F88534735}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{AE4E9BED-A2C1-4836-B34E-75CC6EFF5EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC1B702-DE38-4B03-A090-0A177F45F4E8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>SharepoiintEnergia</t>
+  </si>
+  <si>
+    <t>RPA_Validacao_Substituta</t>
+  </si>
+  <si>
+    <t>Validacao_Substituta</t>
+  </si>
+  <si>
+    <t>Asset responsavel por permitir fazer o regex de substitutas ou não</t>
   </si>
 </sst>
 </file>
@@ -395,9 +404,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -435,7 +444,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -541,7 +550,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -683,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3021,7 +3030,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3210,7 +3219,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>